<commit_message>
Joss Updated excel v2
</commit_message>
<xml_diff>
--- a/Data/Most_frequent_words_from_survey.xlsx
+++ b/Data/Most_frequent_words_from_survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jossmt/AllThingsPython/ML-for-Good-Hackathon/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BC6323-B4FA-854F-AB2D-F634DEF545BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E31D46-82C9-FE49-BC34-B6FB8C851E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16280" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14709,8 +14709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3498"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G192" sqref="G192"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="E207" sqref="E207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14751,7 +14751,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -14768,7 +14768,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -14785,7 +14785,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -14802,7 +14802,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -14819,7 +14819,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -14836,7 +14836,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -14853,7 +14853,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -14870,7 +14870,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -14887,7 +14887,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -14904,7 +14904,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -14921,7 +14921,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -14938,7 +14938,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -14955,7 +14955,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -14972,7 +14972,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -14989,7 +14989,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -15006,7 +15006,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -15023,7 +15023,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -15040,7 +15040,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -15057,7 +15057,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -15074,7 +15074,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -15091,7 +15091,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -15108,7 +15108,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -15125,7 +15125,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -15142,7 +15142,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -15159,7 +15159,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -15176,7 +15176,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -15193,7 +15193,7 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -15210,7 +15210,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -15227,7 +15227,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -15244,7 +15244,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -15261,7 +15261,7 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -15278,7 +15278,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -15295,7 +15295,7 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -15312,7 +15312,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -15329,7 +15329,7 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -15363,7 +15363,7 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -15380,7 +15380,7 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -15414,7 +15414,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -15431,7 +15431,7 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -15448,7 +15448,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -15465,7 +15465,7 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -15482,7 +15482,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -15516,7 +15516,7 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -15533,7 +15533,7 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -15550,7 +15550,7 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -15567,7 +15567,7 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -15584,7 +15584,7 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -15601,7 +15601,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -15618,7 +15618,7 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -15635,7 +15635,7 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -15652,7 +15652,7 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -15703,7 +15703,7 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -15720,7 +15720,7 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -15737,7 +15737,7 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -15754,7 +15754,7 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -15771,7 +15771,7 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -15788,7 +15788,7 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -15805,7 +15805,7 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -15822,7 +15822,7 @@
         <v>0</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -15839,7 +15839,7 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -15856,7 +15856,7 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -15873,7 +15873,7 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -15907,7 +15907,7 @@
         <v>0</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -15924,7 +15924,7 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -15941,7 +15941,7 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -15958,7 +15958,7 @@
         <v>0</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -15975,7 +15975,7 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -15992,7 +15992,7 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -16009,7 +16009,7 @@
         <v>0</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -16026,7 +16026,7 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -16043,7 +16043,7 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -16060,7 +16060,7 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -16077,7 +16077,7 @@
         <v>0</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -16094,7 +16094,7 @@
         <v>0</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -16111,7 +16111,7 @@
         <v>0</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -16128,7 +16128,7 @@
         <v>0</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -16145,7 +16145,7 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -16162,7 +16162,7 @@
         <v>0</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -16179,7 +16179,7 @@
         <v>0</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -16196,7 +16196,7 @@
         <v>0</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -16213,7 +16213,7 @@
         <v>0</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -16230,7 +16230,7 @@
         <v>0</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -16247,7 +16247,7 @@
         <v>0</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -16264,7 +16264,7 @@
         <v>0</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -16298,7 +16298,7 @@
         <v>0</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -16315,7 +16315,7 @@
         <v>0</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -16332,7 +16332,7 @@
         <v>0</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -16349,7 +16349,7 @@
         <v>0</v>
       </c>
       <c r="E96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -16366,7 +16366,7 @@
         <v>0</v>
       </c>
       <c r="E97">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -16383,7 +16383,7 @@
         <v>0</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -16400,7 +16400,7 @@
         <v>0</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -16434,7 +16434,7 @@
         <v>0</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -16451,7 +16451,7 @@
         <v>0</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -16468,7 +16468,7 @@
         <v>0</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -16485,7 +16485,7 @@
         <v>0</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -16502,7 +16502,7 @@
         <v>0</v>
       </c>
       <c r="E105">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -16519,7 +16519,7 @@
         <v>0</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -16536,7 +16536,7 @@
         <v>0</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -16553,7 +16553,7 @@
         <v>0</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -16570,7 +16570,7 @@
         <v>0</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -16587,7 +16587,7 @@
         <v>0</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -16604,7 +16604,7 @@
         <v>0</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -16621,7 +16621,7 @@
         <v>0</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -16638,7 +16638,7 @@
         <v>0</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -16655,7 +16655,7 @@
         <v>0</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -16672,7 +16672,7 @@
         <v>0</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -16689,7 +16689,7 @@
         <v>0</v>
       </c>
       <c r="E116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -16706,7 +16706,7 @@
         <v>0</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -16723,7 +16723,7 @@
         <v>0</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -16740,7 +16740,7 @@
         <v>0</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -16757,7 +16757,7 @@
         <v>0</v>
       </c>
       <c r="E120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -16774,7 +16774,7 @@
         <v>0</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -16791,7 +16791,7 @@
         <v>0</v>
       </c>
       <c r="E122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -16808,7 +16808,7 @@
         <v>0</v>
       </c>
       <c r="E123">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -16825,7 +16825,7 @@
         <v>0</v>
       </c>
       <c r="E124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -16842,7 +16842,7 @@
         <v>0</v>
       </c>
       <c r="E125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -16859,7 +16859,7 @@
         <v>0</v>
       </c>
       <c r="E126">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -16876,7 +16876,7 @@
         <v>0</v>
       </c>
       <c r="E127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -16893,7 +16893,7 @@
         <v>0</v>
       </c>
       <c r="E128">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -16910,7 +16910,7 @@
         <v>0</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -16927,7 +16927,7 @@
         <v>0</v>
       </c>
       <c r="E130">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -16944,7 +16944,7 @@
         <v>0</v>
       </c>
       <c r="E131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -16961,7 +16961,7 @@
         <v>0</v>
       </c>
       <c r="E132">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -16978,7 +16978,7 @@
         <v>0</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -16995,7 +16995,7 @@
         <v>0</v>
       </c>
       <c r="E134">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -17012,7 +17012,7 @@
         <v>0</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -17029,7 +17029,7 @@
         <v>0</v>
       </c>
       <c r="E136">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -17046,7 +17046,7 @@
         <v>0</v>
       </c>
       <c r="E137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -17063,7 +17063,7 @@
         <v>0</v>
       </c>
       <c r="E138">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -17080,7 +17080,7 @@
         <v>0</v>
       </c>
       <c r="E139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -17097,7 +17097,7 @@
         <v>0</v>
       </c>
       <c r="E140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -17114,7 +17114,7 @@
         <v>0</v>
       </c>
       <c r="E141">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -17131,7 +17131,7 @@
         <v>0</v>
       </c>
       <c r="E142">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -17148,7 +17148,7 @@
         <v>0</v>
       </c>
       <c r="E143">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -17165,7 +17165,7 @@
         <v>0</v>
       </c>
       <c r="E144">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -17182,7 +17182,7 @@
         <v>0</v>
       </c>
       <c r="E145">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -17199,7 +17199,7 @@
         <v>0</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -17233,7 +17233,7 @@
         <v>0</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -17250,7 +17250,7 @@
         <v>0</v>
       </c>
       <c r="E149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -17267,7 +17267,7 @@
         <v>0</v>
       </c>
       <c r="E150">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -17284,7 +17284,7 @@
         <v>0</v>
       </c>
       <c r="E151">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -17301,7 +17301,7 @@
         <v>0</v>
       </c>
       <c r="E152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -17318,7 +17318,7 @@
         <v>0</v>
       </c>
       <c r="E153">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -17335,7 +17335,7 @@
         <v>0</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -17352,7 +17352,7 @@
         <v>0</v>
       </c>
       <c r="E155">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -17369,7 +17369,7 @@
         <v>0</v>
       </c>
       <c r="E156">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -17386,7 +17386,7 @@
         <v>0</v>
       </c>
       <c r="E157">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -17403,7 +17403,7 @@
         <v>0</v>
       </c>
       <c r="E158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -17420,7 +17420,7 @@
         <v>0</v>
       </c>
       <c r="E159">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -17437,7 +17437,7 @@
         <v>0</v>
       </c>
       <c r="E160">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -17454,7 +17454,7 @@
         <v>0</v>
       </c>
       <c r="E161">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -17471,7 +17471,7 @@
         <v>0</v>
       </c>
       <c r="E162">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -17488,7 +17488,7 @@
         <v>0</v>
       </c>
       <c r="E163">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -17505,7 +17505,7 @@
         <v>0</v>
       </c>
       <c r="E164">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -17539,7 +17539,7 @@
         <v>0</v>
       </c>
       <c r="E166">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -17556,7 +17556,7 @@
         <v>0</v>
       </c>
       <c r="E167">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -17573,7 +17573,7 @@
         <v>0</v>
       </c>
       <c r="E168">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -17590,7 +17590,7 @@
         <v>0</v>
       </c>
       <c r="E169">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -17607,7 +17607,7 @@
         <v>0</v>
       </c>
       <c r="E170">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -17624,7 +17624,7 @@
         <v>0</v>
       </c>
       <c r="E171">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -17641,7 +17641,7 @@
         <v>0</v>
       </c>
       <c r="E172">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -17658,7 +17658,7 @@
         <v>0</v>
       </c>
       <c r="E173">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -17675,7 +17675,7 @@
         <v>0</v>
       </c>
       <c r="E174">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -17692,7 +17692,7 @@
         <v>0</v>
       </c>
       <c r="E175">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -17709,7 +17709,7 @@
         <v>0</v>
       </c>
       <c r="E176">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -17726,7 +17726,7 @@
         <v>0</v>
       </c>
       <c r="E177">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -17743,7 +17743,7 @@
         <v>0</v>
       </c>
       <c r="E178">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -17760,7 +17760,7 @@
         <v>0</v>
       </c>
       <c r="E179">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
@@ -17777,7 +17777,7 @@
         <v>0</v>
       </c>
       <c r="E180">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
@@ -17794,7 +17794,7 @@
         <v>0</v>
       </c>
       <c r="E181">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -17811,7 +17811,7 @@
         <v>0</v>
       </c>
       <c r="E182">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
@@ -17828,7 +17828,7 @@
         <v>0</v>
       </c>
       <c r="E183">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -17845,7 +17845,7 @@
         <v>0</v>
       </c>
       <c r="E184">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -17862,7 +17862,7 @@
         <v>0</v>
       </c>
       <c r="E185">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
@@ -17879,7 +17879,7 @@
         <v>0</v>
       </c>
       <c r="E186">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
@@ -17896,7 +17896,7 @@
         <v>0</v>
       </c>
       <c r="E187">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
@@ -17913,7 +17913,7 @@
         <v>0</v>
       </c>
       <c r="E188">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
@@ -17930,7 +17930,7 @@
         <v>0</v>
       </c>
       <c r="E189">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
@@ -17947,7 +17947,7 @@
         <v>0</v>
       </c>
       <c r="E190">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -17964,7 +17964,7 @@
         <v>0</v>
       </c>
       <c r="E191">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -17981,7 +17981,7 @@
         <v>0</v>
       </c>
       <c r="E192">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -17998,7 +17998,7 @@
         <v>0</v>
       </c>
       <c r="E193">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -18015,7 +18015,7 @@
         <v>0</v>
       </c>
       <c r="E194">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -18032,7 +18032,7 @@
         <v>0</v>
       </c>
       <c r="E195">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
@@ -18049,7 +18049,7 @@
         <v>0</v>
       </c>
       <c r="E196">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
@@ -18066,7 +18066,7 @@
         <v>0</v>
       </c>
       <c r="E197">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
@@ -18083,7 +18083,7 @@
         <v>0</v>
       </c>
       <c r="E198">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -18100,7 +18100,7 @@
         <v>0</v>
       </c>
       <c r="E199">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
@@ -18117,7 +18117,7 @@
         <v>0</v>
       </c>
       <c r="E200">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
@@ -18134,7 +18134,7 @@
         <v>0</v>
       </c>
       <c r="E201">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>